<commit_message>
Henry Buck plant data linear models phase 1.
</commit_message>
<xml_diff>
--- a/Data/2017 henry buck trail plant community plots.xlsx
+++ b/Data/2017 henry buck trail plant community plots.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\OneDrive - Washington State University (email.wsu.edu)\Henry Buck Trail Experiment\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailwsu-my.sharepoint.com/personal/robert_e_clark_wsu_edu/Documents/Henry-Buck-Trail-Experiment/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96A2FBE7-997D-4B41-8DBC-012D9CA13BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{96A2FBE7-997D-4B41-8DBC-012D9CA13BC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4E0E219-32C1-41C3-888B-AA757749F424}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,93 +31,30 @@
     <t>Mayflower</t>
   </si>
   <si>
-    <t>Trout lily</t>
-  </si>
-  <si>
     <t>Violet</t>
   </si>
   <si>
     <t>Trillium</t>
   </si>
   <si>
-    <t>D breeches</t>
-  </si>
-  <si>
     <t>Toothwort</t>
   </si>
   <si>
-    <t>ginseng</t>
-  </si>
-  <si>
-    <t>anemone</t>
-  </si>
-  <si>
-    <t>jewelweed</t>
-  </si>
-  <si>
-    <t>cinquefoil</t>
-  </si>
-  <si>
-    <t>wood aster</t>
-  </si>
-  <si>
-    <t>carex</t>
-  </si>
-  <si>
-    <t>starflower</t>
-  </si>
-  <si>
-    <t>blue cohosh</t>
-  </si>
-  <si>
-    <t>Indian Cucumber</t>
-  </si>
-  <si>
-    <t>Foam Flower</t>
-  </si>
-  <si>
     <t>Hepatica</t>
   </si>
   <si>
-    <t>Solomons Seal</t>
-  </si>
-  <si>
     <t>Jumpseed</t>
   </si>
   <si>
     <t>Cleavers</t>
   </si>
   <si>
-    <t>Fern Plant</t>
-  </si>
-  <si>
-    <t>Carrot</t>
-  </si>
-  <si>
-    <t>Yellow Violet</t>
-  </si>
-  <si>
-    <t>House Plant Flower</t>
-  </si>
-  <si>
     <t>Bloodroot</t>
   </si>
   <si>
     <t>Allium</t>
   </si>
   <si>
-    <t>Stinging Nettle</t>
-  </si>
-  <si>
-    <t>Wide Carex</t>
-  </si>
-  <si>
-    <t>fuzzy plant</t>
-  </si>
-  <si>
-    <t>Spring beauty</t>
-  </si>
-  <si>
     <t>Control</t>
   </si>
   <si>
@@ -128,6 +65,69 @@
   </si>
   <si>
     <t>Treatment_2017</t>
+  </si>
+  <si>
+    <t>Spring_beauty</t>
+  </si>
+  <si>
+    <t>Trout_lily</t>
+  </si>
+  <si>
+    <t>D_breeches</t>
+  </si>
+  <si>
+    <t>Ginseng</t>
+  </si>
+  <si>
+    <t>Anemone</t>
+  </si>
+  <si>
+    <t>Jewelweed</t>
+  </si>
+  <si>
+    <t>Cinquefoil</t>
+  </si>
+  <si>
+    <t>Wood_aster</t>
+  </si>
+  <si>
+    <t>Carex</t>
+  </si>
+  <si>
+    <t>Starflower</t>
+  </si>
+  <si>
+    <t>Blue_cohosh</t>
+  </si>
+  <si>
+    <t>Indian_cucumber</t>
+  </si>
+  <si>
+    <t>Foamflower</t>
+  </si>
+  <si>
+    <t>Solomon_seal</t>
+  </si>
+  <si>
+    <t>Fern_plant</t>
+  </si>
+  <si>
+    <t>Carrot_sp</t>
+  </si>
+  <si>
+    <t>Yellow_violet</t>
+  </si>
+  <si>
+    <t>house_plant_flower</t>
+  </si>
+  <si>
+    <t>Stinging_nettle</t>
+  </si>
+  <si>
+    <t>Wide_carex</t>
+  </si>
+  <si>
+    <t>Fuzzy_plant</t>
   </si>
 </sst>
 </file>
@@ -487,9 +487,9 @@
   </sheetPr>
   <dimension ref="A1:AG118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="AG1" sqref="AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -505,97 +505,97 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -606,7 +606,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="H2" s="1">
         <v>10</v>
@@ -623,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1">
         <v>16</v>
@@ -637,7 +637,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1">
         <v>10</v>
@@ -654,7 +654,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D5" s="1">
         <v>2</v>
@@ -674,7 +674,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1">
         <v>12</v>
@@ -694,7 +694,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D7" s="1">
         <v>8</v>
@@ -720,7 +720,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D8" s="1">
         <v>6</v>
@@ -746,7 +746,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D9" s="1">
         <v>28</v>
@@ -772,7 +772,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D10" s="1">
         <v>29</v>
@@ -795,7 +795,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D11" s="1">
         <v>16</v>
@@ -818,7 +818,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D12" s="1">
         <v>2</v>
@@ -841,7 +841,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -852,7 +852,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -863,7 +863,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D15" s="1">
         <v>6</v>
@@ -889,7 +889,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D16" s="1">
         <v>16</v>
@@ -909,7 +909,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
@@ -929,7 +929,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D18" s="1">
         <v>3</v>
@@ -949,7 +949,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="E19" s="1">
         <v>3</v>
@@ -966,7 +966,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D20" s="1">
         <v>2</v>
@@ -986,7 +986,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D21" s="1">
         <v>2</v>
@@ -1006,7 +1006,7 @@
         <v>2</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D22" s="1">
         <v>5</v>
@@ -1026,7 +1026,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D23" s="1">
         <v>17</v>
@@ -1049,7 +1049,7 @@
         <v>2</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D24" s="1">
         <v>17</v>
@@ -1069,7 +1069,7 @@
         <v>2</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D25" s="1">
         <v>25</v>
@@ -1089,7 +1089,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="E26" s="1">
         <v>3</v>
@@ -1109,7 +1109,7 @@
         <v>2</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="13.2" x14ac:dyDescent="0.25">
@@ -1120,7 +1120,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D28" s="1">
         <v>21</v>
@@ -1137,7 +1137,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
@@ -1157,7 +1157,7 @@
         <v>3</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D30" s="1">
         <v>31</v>
@@ -1177,7 +1177,7 @@
         <v>3</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D31" s="1">
         <v>20</v>
@@ -1197,7 +1197,7 @@
         <v>3</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D32" s="1">
         <v>27</v>
@@ -1220,7 +1220,7 @@
         <v>3</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D33" s="1">
         <v>16</v>
@@ -1240,7 +1240,7 @@
         <v>3</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D34" s="1">
         <v>19</v>
@@ -1260,7 +1260,7 @@
         <v>3</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D35" s="1">
         <v>12</v>
@@ -1286,7 +1286,7 @@
         <v>3</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D36" s="1">
         <v>10</v>
@@ -1309,7 +1309,7 @@
         <v>3</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D37" s="1">
         <v>20</v>
@@ -1338,7 +1338,7 @@
         <v>3</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="E38" s="1">
         <v>23</v>
@@ -1364,7 +1364,7 @@
         <v>3</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D39" s="1">
         <v>3</v>
@@ -1387,7 +1387,7 @@
         <v>3</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41" spans="1:22" ht="13.2" x14ac:dyDescent="0.25">
@@ -1398,7 +1398,7 @@
         <v>4</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D41" s="1">
         <v>5</v>
@@ -1415,7 +1415,7 @@
         <v>4</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D42" s="1">
         <v>15</v>
@@ -1432,7 +1432,7 @@
         <v>4</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D43" s="1">
         <v>21</v>
@@ -1449,7 +1449,7 @@
         <v>4</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D44" s="1">
         <v>28</v>
@@ -1466,7 +1466,7 @@
         <v>4</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D45" s="1">
         <v>21</v>
@@ -1486,7 +1486,7 @@
         <v>4</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D46" s="1">
         <v>17</v>
@@ -1503,7 +1503,7 @@
         <v>4</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D47" s="1">
         <v>12</v>
@@ -1523,7 +1523,7 @@
         <v>4</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D48" s="1">
         <v>28</v>
@@ -1543,7 +1543,7 @@
         <v>4</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D49" s="1">
         <v>26</v>
@@ -1563,7 +1563,7 @@
         <v>4</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D50" s="1">
         <v>14</v>
@@ -1592,7 +1592,7 @@
         <v>4</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D51" s="1">
         <v>19</v>
@@ -1615,7 +1615,7 @@
         <v>4</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D52" s="1">
         <v>8</v>
@@ -1632,7 +1632,7 @@
         <v>4</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:24" ht="13.2" x14ac:dyDescent="0.25">
@@ -1643,7 +1643,7 @@
         <v>5</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D54" s="1">
         <v>4</v>
@@ -1666,7 +1666,7 @@
         <v>5</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D55" s="1">
         <v>3</v>
@@ -1686,7 +1686,7 @@
         <v>5</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D56" s="1">
         <v>3</v>
@@ -1709,7 +1709,7 @@
         <v>5</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D57" s="1">
         <v>24</v>
@@ -1732,7 +1732,7 @@
         <v>5</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D58" s="1">
         <v>18</v>
@@ -1752,7 +1752,7 @@
         <v>5</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D59" s="1">
         <v>39</v>
@@ -1775,7 +1775,7 @@
         <v>5</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D60" s="1">
         <v>21</v>
@@ -1798,7 +1798,7 @@
         <v>5</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D61" s="1">
         <v>5</v>
@@ -1818,7 +1818,7 @@
         <v>5</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D62" s="1">
         <v>9</v>
@@ -1841,7 +1841,7 @@
         <v>5</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D63" s="1">
         <v>10</v>
@@ -1864,7 +1864,7 @@
         <v>5</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D64" s="1">
         <v>29</v>
@@ -1890,7 +1890,7 @@
         <v>5</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D65" s="1">
         <v>15</v>
@@ -1913,7 +1913,7 @@
         <v>5</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="67" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
@@ -1924,7 +1924,7 @@
         <v>6</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D67" s="1">
         <v>2</v>
@@ -1947,7 +1947,7 @@
         <v>6</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D68" s="1">
         <v>35</v>
@@ -1973,7 +1973,7 @@
         <v>6</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D69" s="1">
         <v>12</v>
@@ -1999,7 +1999,7 @@
         <v>6</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D70" s="1">
         <v>14</v>
@@ -2034,7 +2034,7 @@
         <v>6</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D71" s="1">
         <v>31</v>
@@ -2063,7 +2063,7 @@
         <v>6</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D72" s="1">
         <v>14</v>
@@ -2092,7 +2092,7 @@
         <v>6</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D73" s="1">
         <v>33</v>
@@ -2124,7 +2124,7 @@
         <v>6</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D74" s="1">
         <v>41</v>
@@ -2144,7 +2144,7 @@
         <v>6</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D75" s="1">
         <v>65</v>
@@ -2164,7 +2164,7 @@
         <v>6</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D76" s="1">
         <v>28</v>
@@ -2187,7 +2187,7 @@
         <v>6</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D77" s="1">
         <v>25</v>
@@ -2213,7 +2213,7 @@
         <v>6</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D78" s="1">
         <v>14</v>
@@ -2233,7 +2233,7 @@
         <v>6</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="80" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
@@ -2244,7 +2244,7 @@
         <v>7</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D80" s="1">
         <v>26</v>
@@ -2264,7 +2264,7 @@
         <v>7</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D81" s="1">
         <v>36</v>
@@ -2284,7 +2284,7 @@
         <v>7</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D82" s="1">
         <v>24</v>
@@ -2310,7 +2310,7 @@
         <v>7</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D83" s="1">
         <v>36</v>
@@ -2333,7 +2333,7 @@
         <v>7</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D84" s="1">
         <v>36</v>
@@ -2362,7 +2362,7 @@
         <v>7</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D85" s="1">
         <v>15</v>
@@ -2394,7 +2394,7 @@
         <v>7</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D86" s="1">
         <v>18</v>
@@ -2429,7 +2429,7 @@
         <v>7</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D87" s="1">
         <v>11</v>
@@ -2469,7 +2469,7 @@
         <v>7</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D88" s="1">
         <v>20</v>
@@ -2510,7 +2510,7 @@
         <v>7</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D89" s="1">
         <v>36</v>
@@ -2542,7 +2542,7 @@
         <v>7</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D90" s="1">
         <v>40</v>
@@ -2571,7 +2571,7 @@
         <v>7</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="D91" s="1">
         <v>31</v>
@@ -2597,7 +2597,7 @@
         <v>7</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="93" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
@@ -2608,7 +2608,7 @@
         <v>8</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="H93" s="1">
         <v>9</v>
@@ -2622,7 +2622,7 @@
         <v>8</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D94" s="1">
         <v>36</v>
@@ -2645,7 +2645,7 @@
         <v>8</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D95" s="1">
         <v>38</v>
@@ -2668,7 +2668,7 @@
         <v>8</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D96" s="1">
         <v>17</v>
@@ -2691,7 +2691,7 @@
         <v>8</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D97" s="1">
         <v>9</v>
@@ -2714,7 +2714,7 @@
         <v>8</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D98" s="1">
         <v>9</v>
@@ -2734,7 +2734,7 @@
         <v>8</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="G99" s="1">
         <v>23</v>
@@ -2759,7 +2759,7 @@
         <v>8</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="G100" s="1">
         <v>15</v>
@@ -2779,7 +2779,7 @@
         <v>8</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D101" s="1">
         <v>9</v>
@@ -2802,7 +2802,7 @@
         <v>8</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D102" s="1">
         <v>43</v>
@@ -2828,7 +2828,7 @@
         <v>8</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D103" s="1">
         <v>48</v>
@@ -2855,7 +2855,7 @@
         <v>8</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="D104" s="1">
         <v>6</v>
@@ -2879,7 +2879,7 @@
         <v>8</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
     </row>
     <row r="106" spans="1:33" ht="13.2" x14ac:dyDescent="0.25">
@@ -2890,7 +2890,7 @@
         <v>9</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D106" s="1">
         <v>13</v>
@@ -2913,7 +2913,7 @@
         <v>9</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D107" s="1">
         <v>14</v>
@@ -2936,7 +2936,7 @@
         <v>9</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D108" s="1">
         <v>13</v>
@@ -2962,7 +2962,7 @@
         <v>9</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D109" s="1">
         <v>21</v>
@@ -2991,7 +2991,7 @@
         <v>9</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D110" s="1">
         <v>12</v>
@@ -3017,7 +3017,7 @@
         <v>9</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D111" s="1">
         <v>23</v>
@@ -3046,7 +3046,7 @@
         <v>9</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D112" s="1">
         <v>13</v>
@@ -3072,7 +3072,7 @@
         <v>9</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D113" s="1">
         <v>37</v>
@@ -3101,7 +3101,7 @@
         <v>9</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D114" s="1">
         <v>37</v>
@@ -3143,7 +3143,7 @@
         <v>9</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="H115" s="1">
         <v>8</v>
@@ -3169,7 +3169,7 @@
         <v>9</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D116" s="1">
         <v>20</v>
@@ -3198,7 +3198,7 @@
         <v>9</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="D117" s="1">
         <v>19</v>
@@ -3236,7 +3236,7 @@
         <v>9</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>